<commit_message>
Add ppt file for Q1A for Question Set 1
</commit_message>
<xml_diff>
--- a/csv-files/top-10-animation-movies.xlsx
+++ b/csv-files/top-10-animation-movies.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="top10-animation-hbarchart1" sheetId="2" r:id="rId1"/>
     <sheet name="top-10-animation-movies" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -745,11 +745,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="86993152"/>
-        <c:axId val="86994944"/>
+        <c:axId val="39746944"/>
+        <c:axId val="39748736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86993152"/>
+        <c:axId val="39746944"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -758,7 +758,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86994944"/>
+        <c:crossAx val="39748736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -766,7 +766,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86994944"/>
+        <c:axId val="39748736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +800,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86993152"/>
+        <c:crossAx val="39746944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>